<commit_message>
Se corregio la palabra
</commit_message>
<xml_diff>
--- a/public/reportes/reporteCombinado.xlsx
+++ b/public/reportes/reporteCombinado.xlsx
@@ -179,7 +179,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>07-07-2022 12:22:48 pm</t>
+          <t>07-08-2022 12:02:25 pm</t>
         </is>
       </c>
       <c r="K12" s="3" t="inlineStr">
@@ -458,7 +458,7 @@
       </c>
       <c r="AA15" s="1" t="inlineStr">
         <is>
-          <t>Total acomulado</t>
+          <t>Total acumulado</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="O17" s="0" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>133</t>
         </is>
       </c>
       <c r="P17" s="0" t="inlineStr">
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="AA17" s="0">
-        <v>10</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insert de valores de variables y reporte de variables
</commit_message>
<xml_diff>
--- a/public/reportes/reporteCombinado.xlsx
+++ b/public/reportes/reporteCombinado.xlsx
@@ -215,7 +215,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>11-07-2022 03:40:22 pm</t>
+          <t>11-11-2022 03:06:38 pm</t>
         </is>
       </c>
       <c r="K12" s="2" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="K16" s="0" t="inlineStr">
         <is>
-          <t>Número de acciones realizadas del Programa para mitigar las emisiones de gases de efecto invernadero y la huella de carbono del sector energético,Totales de acciones programadas del Programa para mitigar las emisiones de gases de efecto invernadero y la huella de carbono del sector energético,100</t>
+          <t>Totales de acciones programadas del Programa para mitigar las emisiones de gases de efecto invernadero y la huella de carbono del sector energético,100,Número de acciones realizadas del Programa para mitigar las emisiones de gases de efecto invernadero y la huella de carbono del sector energético</t>
         </is>
       </c>
       <c r="L16" s="0" t="inlineStr">
@@ -569,32 +569,44 @@
           <t>Número de proyectos convenidos o contratados</t>
         </is>
       </c>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3">
+        <v>20</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0</v>
+      </c>
       <c r="AA16" s="3">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -620,84 +632,758 @@
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
+          <t>3.2.2.-  Implementar un programa de educación, capacitacion y concientización en materia de eficiencia energética.</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>4777</t>
+        </is>
+      </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de avance de acciones realizadas para el programa de educación, capacitacion y concientización en materia de eficiencia energética con respecto al total de acciones a realizar.</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="J17" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+      <c r="K17" s="0" t="inlineStr">
+        <is>
+          <t>100,Número de acciones realizadas del programa de educación, apacitacion y concientización en materia de eficiencia energética.,Total de acciones a realizar</t>
+        </is>
+      </c>
+      <c r="L17" s="0" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="M17" s="0" t="inlineStr">
+        <is>
+          <t>(A/B)*C</t>
+        </is>
+      </c>
+      <c r="N17" s="0" t="inlineStr">
+        <is>
+          <t>Firma de  convenio con UNECE para lanzamiento del programa</t>
+        </is>
+      </c>
+      <c r="O17" s="3">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="3">
+        <v>20</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0</v>
+      </c>
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>4.4.4.2 Promover el acceso y el uso eficiente de la energía, con énfasis en las energías renovables.</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>gestion</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>Eficacia</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
           <t>3.2.3.-  Desarrollar programas de ahorro de energía en el sector público.</t>
         </is>
       </c>
-      <c r="F17" s="0" t="inlineStr">
+      <c r="F18" s="0" t="inlineStr">
         <is>
           <t>4778</t>
         </is>
       </c>
-      <c r="G17" s="0" t="inlineStr">
+      <c r="G18" s="0" t="inlineStr">
         <is>
           <t>Porcentaje de programas realizados para el ahorro de energía en el sector público con respecto al total de programas a realizar</t>
         </is>
       </c>
-      <c r="H17" s="0" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="I17" s="0" t="inlineStr">
+      <c r="H18" s="0" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I18" s="0" t="inlineStr">
         <is>
           <t>Trimestral</t>
         </is>
       </c>
-      <c r="J17" s="0" t="inlineStr">
+      <c r="J18" s="0" t="inlineStr">
         <is>
           <t>Porcentaje</t>
         </is>
       </c>
-      <c r="K17" s="0" t="inlineStr">
-        <is>
-          <t>Número de programas realizados para el ahorro de energía en el sector público,100,Total de programas a realizar | Total de programas a realizar,Número de programas realizados para el ahorro de energía en el sector público,100</t>
-        </is>
-      </c>
-      <c r="L17" s="0" t="inlineStr">
+      <c r="K18" s="0" t="inlineStr">
+        <is>
+          <t>100,Número de programas realizados para el ahorro de energía en el sector público,Total de programas a realizar</t>
+        </is>
+      </c>
+      <c r="L18" s="0" t="inlineStr">
         <is>
           <t>Porcentaje de Avance</t>
         </is>
       </c>
-      <c r="M17" s="0" t="inlineStr">
+      <c r="M18" s="0" t="inlineStr">
+        <is>
+          <t>(B/D)*E</t>
+        </is>
+      </c>
+      <c r="N18" s="0" t="inlineStr">
+        <is>
+          <t>Publicación en redes sociales</t>
+        </is>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="3">
+        <v>20</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>4.4.4.2 Promover el acceso y el uso eficiente de la energía, con énfasis en las energías renovables.</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>gestion</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>Eficacia</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>4.1.2.-  Promover e implementar proyectos de generación eléctrica a partir del aprovechamiento de energías renovables</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>4782</t>
+        </is>
+      </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de avance de proyectos implementados de generación eléctrica con respecto al total proyectos a implementar.</t>
+        </is>
+      </c>
+      <c r="H19" s="0" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I19" s="0" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="J19" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+      <c r="K19" s="0" t="inlineStr">
+        <is>
+          <t>Número de proyectos implementados de generación eléctrica,100,Total proyectos a implementar</t>
+        </is>
+      </c>
+      <c r="L19" s="0" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="M19" s="0" t="inlineStr">
         <is>
           <t>(A/B)*C</t>
         </is>
       </c>
-      <c r="N17" s="0" t="inlineStr">
-        <is>
-          <t>Publicación en redes sociales</t>
-        </is>
-      </c>
-      <c r="O17" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3" t="inlineStr">
-        <is>
-          <t>33.3</t>
-        </is>
-      </c>
-      <c r="S17" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="T17" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3">
-        <v>35.3</v>
+      <c r="N19" s="0" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="3">
+        <v>33.33</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>4.4.4.2 Promover el acceso y el uso eficiente de la energía, con énfasis en las energías renovables.</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>gestion</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>Eficacia</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>Crear un Fideicomiso para el desarrollo energético sustentable que permita financiar la  implementación de programas y proyectos en el  Estado de Querétaro.</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>5597</t>
+        </is>
+      </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de etapas concluidas en la creación del Fideicomiso para el Desarrollo Energético Sustentable respecto del total de etapas programadas</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="J20" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+      <c r="K20" s="0" t="inlineStr">
+        <is>
+          <t>Total de etapas programadas,Número de etapas concluidas en la creación del Fideicomiso para el Desarrollo Energético Sustentable,100</t>
+        </is>
+      </c>
+      <c r="L20" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de Avance</t>
+        </is>
+      </c>
+      <c r="M20" s="0" t="inlineStr">
+        <is>
+          <t>(A/B)*C</t>
+        </is>
+      </c>
+      <c r="N20" s="0" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0</v>
+      </c>
+      <c r="T20" s="3">
+        <v>20</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>4.4.4.2 Promover el acceso y el uso eficiente de la energía, con énfasis en las energías renovables.</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>gestion</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>Eficacia</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>Promover proyectos de generación distribuída y abasto aislado de electricidad en edificios públicos.</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>5598</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de avance de acciones para la generación distribuída y de abasto aislado de electricidad en edificios públicos con respecto al total de acciones .</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>Trimestral</t>
+        </is>
+      </c>
+      <c r="J21" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+      <c r="K21" s="0" t="inlineStr">
+        <is>
+          <t>Acciones RealizadasNúmero de acciones realizadas para la generación distribuída y de abasto aislado de electricidad en edificios públicos,Total de acciones programadas para la generación distribuida y abasto en edificios públicos,100</t>
+        </is>
+      </c>
+      <c r="L21" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de Avance</t>
+        </is>
+      </c>
+      <c r="M21" s="0" t="inlineStr">
+        <is>
+          <t>(A/B)*C</t>
+        </is>
+      </c>
+      <c r="N21" s="0" t="inlineStr">
+        <is>
+          <t>Convenio con empresa para promover celdas solares</t>
+        </is>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>100</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3">
+        <v>0</v>
+      </c>
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>4.4.3.2 Ampliar el sistema de distribución de energía eléctrica.</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>gestion</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>Eficiencia</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>2.1.3.- Integrar un portafolio de proyectos de energía competitivo que atraiga la inversión a Querétaro.</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>5650</t>
+        </is>
+      </c>
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje de avance de acciones realizadas para integrar el portafolio de proyectos de energía con respecto a las acciones a realizar.</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t>Trimestral</t>
+        </is>
+      </c>
+      <c r="J22" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+      <c r="K22" s="0" t="inlineStr">
+        <is>
+          <t>Número acciones realizadas para integrar el portafolio de proyectos de energía,100,Totales del acciones a realizar</t>
+        </is>
+      </c>
+      <c r="L22" s="0" t="inlineStr">
+        <is>
+          <t>Porcentaje</t>
+        </is>
+      </c>
+      <c r="M22" s="0" t="inlineStr">
+        <is>
+          <t>(A/B)*C</t>
+        </is>
+      </c>
+      <c r="N22" s="0" t="inlineStr">
+        <is>
+          <t>Proejecución de ejecución de polo de desarrollo aeropuerto </t>
+        </is>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>30</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0</v>
+      </c>
+      <c r="W22" s="3">
+        <v>0</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>Actividad</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>4.4.3.1 Desarrollar redes de autoabasto eléctrico.</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>gestion</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>Eficacia</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>2.4.2.-  Construir e instalar infraestructura energetica</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>5654</t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>Sumatoria de extensiones de líneas de alta tensión instaladas</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
+        <is>
+          <t>Sumatoria</t>
+        </is>
+      </c>
+      <c r="K23" s="0" t="inlineStr">
+        <is>
+          <t>C, Número de extensiones de líneas de alta tensión instaladas,B</t>
+        </is>
+      </c>
+      <c r="L23" s="0" t="inlineStr">
+        <is>
+          <t>Línea</t>
+        </is>
+      </c>
+      <c r="M23" s="0" t="inlineStr">
+        <is>
+          <t>(A/B)*C</t>
+        </is>
+      </c>
+      <c r="N23" s="0" t="inlineStr">
+        <is>
+          <t>Proejecución de ejecución de polo de desarrollo aeropuerto </t>
+        </is>
+      </c>
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="3">
+        <v>25</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <v>0</v>
+      </c>
+      <c r="W23" s="3">
+        <v>0</v>
+      </c>
+      <c r="X23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>